<commit_message>
new files, changing email server to localhost
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredmathew/PythonStuff/Email-Sender/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76046655-6CB6-1241-9802-B27E11C9E5EC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE917FE4-FEA1-4945-BFC6-CAAE5F49EB9B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18160" windowHeight="14500" xr2:uid="{945A9013-496A-45AA-A316-483B626892D7}"/>
   </bookViews>
@@ -19,12 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -809,7 +803,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -970,7 +964,7 @@
         <v>43018</v>
       </c>
       <c r="D4" s="3">
-        <v>43079</v>
+        <v>43095</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>

</xml_diff>